<commit_message>
Implement first version of Generic Test case, add setting properties to object as it would be a tree
</commit_message>
<xml_diff>
--- a/NUnitTest/TestSample.xlsx
+++ b/NUnitTest/TestSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKonicki\source\repos\ExcelTest\ExcelTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKonicki\Documents\Prywatne\DDT-TEST\NUnitTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A94C3AF-24F7-4377-AB99-2FE8C820526E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367EE117-7ED1-4C65-9F7B-B64B24A72739}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4C03CD2C-4807-4FF8-9699-637F3855A9BA}"/>
   </bookViews>
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA39F5D-E458-4BD8-B62F-814354E1D7E7}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>